<commit_message>
Added C interview questions and materials
</commit_message>
<xml_diff>
--- a/SPI_Data_Worksheet.xlsx
+++ b/SPI_Data_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec11bca0e4bee75f/Desktop/AVR Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10644B0F-9E56-48D4-B5B5-69E057A508DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{10644B0F-9E56-48D4-B5B5-69E057A508DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52FD5445-81CB-453D-810B-05E2214AB422}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{206288DB-9415-474F-A227-6B7981E1625C}"/>
+    <workbookView minimized="1" xWindow="384" yWindow="384" windowWidth="10680" windowHeight="10212" xr2:uid="{206288DB-9415-474F-A227-6B7981E1625C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>FA</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>MSB|LSB|XLSB</t>
+  </si>
+  <si>
+    <t>20 Bit data</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,6 +523,9 @@
       <c r="T1" s="1">
         <v>0</v>
       </c>
+      <c r="W1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="M6" s="2">

</xml_diff>